<commit_message>
lab_1 bugfix, report update, tests added
</commit_message>
<xml_diff>
--- a/lab_1/Report.xlsx
+++ b/lab_1/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shust\Desktop\AOP_cource\lab_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48753BD4-10B6-4FBD-BFD2-ED668B377AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FE284F-4B92-4DA7-8FE2-31697D539351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="2655" windowWidth="24870" windowHeight="15045" xr2:uid="{EF78F52D-0B32-4C85-B6D6-63D670A0ABEE}"/>
   </bookViews>
@@ -140,10 +140,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="181" formatCode="0.00000000000000000000"/>
-    <numFmt numFmtId="182" formatCode="0.000000000000000000000"/>
-    <numFmt numFmtId="184" formatCode="0.00000000000000000000000"/>
-    <numFmt numFmtId="185" formatCode="0.000000000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000000000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -400,16 +400,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="184" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="185" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -423,24 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,6 +440,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -776,7 +776,7 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,30 +786,30 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="2:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="31" t="s">
         <v>4</v>
       </c>
     </row>
@@ -975,30 +975,30 @@
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="14" spans="2:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
         <v>600</v>
       </c>
       <c r="E19" s="19">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="F19" s="19">
         <v>633</v>
@@ -1113,7 +1113,7 @@
         <v>611</v>
       </c>
       <c r="E20" s="19">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F20" s="19">
         <v>695</v>
@@ -1133,7 +1133,7 @@
         <v>1630</v>
       </c>
       <c r="E21" s="19">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="F21" s="19">
         <v>2070</v>
@@ -1153,7 +1153,7 @@
         <v>9523</v>
       </c>
       <c r="E22" s="22">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="F22" s="22">
         <v>9614</v>

</xml_diff>